<commit_message>
cambios en preparación, indicadores y modelo
</commit_message>
<xml_diff>
--- a/Variables.xlsx
+++ b/Variables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natal\Desktop\CEPAL_2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6E51D5F-323D-4EF7-8FAE-87DB385FD94F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D65625F-C8B7-48E0-9629-0C7EE24570B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="38">
   <si>
     <t xml:space="preserve">Variable </t>
   </si>
@@ -120,9 +120,6 @@
     <t>Confianza en las Instituciones</t>
   </si>
   <si>
-    <t>c08_11</t>
-  </si>
-  <si>
     <t>c12_01-; c12_09</t>
   </si>
   <si>
@@ -142,6 +139,15 @@
   </si>
   <si>
     <t>Expectativas de la Movilidad Social</t>
+  </si>
+  <si>
+    <t>listo</t>
+  </si>
+  <si>
+    <t>no disponible</t>
+  </si>
+  <si>
+    <t>c18_11</t>
   </si>
 </sst>
 </file>
@@ -469,7 +475,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -493,7 +499,7 @@
         <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -501,7 +507,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -522,7 +528,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B6" t="s">
         <v>26</v>
@@ -537,8 +543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{805B5725-8824-4874-A9EC-3C44DE592EEF}">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView topLeftCell="A4" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -561,6 +567,9 @@
       <c r="B2" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -569,6 +578,9 @@
       <c r="B3" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="C3" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -577,15 +589,20 @@
       <c r="B4" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="C4" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="1"/>
+      <c r="C5" s="1" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -594,7 +611,9 @@
       <c r="B6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="1"/>
+      <c r="C6" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -603,7 +622,9 @@
       <c r="B7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="1"/>
+      <c r="C7" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -612,23 +633,27 @@
       <c r="B8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="1"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C8" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" s="1"/>
+        <v>29</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C10" s="1"/>
     </row>
@@ -637,7 +662,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C11" s="1"/>
     </row>

</xml_diff>